<commit_message>
added second name in test file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -6,15 +6,24 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="test" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>ime</t>
+    <t>Jelena</t>
+  </si>
+  <si>
+    <t>Vasilijevic</t>
+  </si>
+  <si>
+    <t>Pera</t>
+  </si>
+  <si>
+    <t>Peric</t>
   </si>
 </sst>
 </file>
@@ -59,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -69,6 +78,17 @@
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
added fake data in test file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Jelena</t>
   </si>
@@ -24,6 +24,54 @@
   </si>
   <si>
     <t>Peric</t>
+  </si>
+  <si>
+    <t>Patrina</t>
+  </si>
+  <si>
+    <t>Kuhic</t>
+  </si>
+  <si>
+    <t>Lauran</t>
+  </si>
+  <si>
+    <t>Kovacek</t>
+  </si>
+  <si>
+    <t>Dale</t>
+  </si>
+  <si>
+    <t>Wintheiser</t>
+  </si>
+  <si>
+    <t>Ike</t>
+  </si>
+  <si>
+    <t>Mertz</t>
+  </si>
+  <si>
+    <t>Thurman</t>
+  </si>
+  <si>
+    <t>Mosciski</t>
+  </si>
+  <si>
+    <t>Rigoberto</t>
+  </si>
+  <si>
+    <t>Stroman</t>
+  </si>
+  <si>
+    <t>Rocco</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Hank</t>
+  </si>
+  <si>
+    <t>Cronin</t>
   </si>
 </sst>
 </file>
@@ -68,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -90,6 +138,70 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>